<commit_message>
Add 1 more device
</commit_message>
<xml_diff>
--- a/Interface_Configuration.xlsx
+++ b/Interface_Configuration.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sathanas/Desktop/Accelerators/DevOps/Version_Control/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sathanas/gittest/Version_Control/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED0D2E5-CB2E-B848-A028-09B619F12C6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A453F4D6-20C7-7040-B862-825C206846EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{C4A53B53-F3DA-7644-A5E6-39C4DB3B1B5F}"/>
+    <workbookView xWindow="2940" yWindow="25980" windowWidth="28040" windowHeight="17440" xr2:uid="{C4A53B53-F3DA-7644-A5E6-39C4DB3B1B5F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="48">
   <si>
     <t>Device</t>
   </si>
@@ -174,6 +174,12 @@
   </si>
   <si>
     <t>DOWN</t>
+  </si>
+  <si>
+    <t>NX-OS-21</t>
+  </si>
+  <si>
+    <t>GigabitEthernet 0/0/20</t>
   </si>
 </sst>
 </file>
@@ -229,10 +235,10 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -552,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E72ED99-05D0-B24A-AAA9-014A2C3F4190}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -564,13 +570,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
@@ -578,288 +584,302 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
       <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>22</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>23</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>24</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>25</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>26</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>27</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>28</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
         <v>29</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
         <v>30</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="1">
         <v>31</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="1">
         <v>32</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <v>33</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="1">
         <v>34</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="1">
         <v>35</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="1">
         <v>36</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="1">
         <v>37</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="1">
         <v>38</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="1">
         <v>39</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="1">
         <v>40</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="1">
         <v>41</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="1">
+        <v>41</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>